<commit_message>
add report and update cases
</commit_message>
<xml_diff>
--- a/TestData/Officemate.xlsx
+++ b/TestData/Officemate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DCG\Documents\officemate\linhtt1_qa_automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DCG\Documents\Smart\linhtt1_qa_automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CA255D-88EC-4FFB-A5B8-1CED8B51F0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71D1723-073A-416B-AAC5-975D72F9B4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assumsion" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="102">
   <si>
     <t>Categories</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>zxcvbnmasdfgh</t>
-  </si>
-  <si>
-    <t>ไม่ได้อยู่</t>
   </si>
   <si>
     <t>fdfdf%$@&amp;^</t>
@@ -212,9 +209,6 @@
 Response body</t>
   </si>
   <si>
-    <t>nawaKa</t>
-  </si>
-  <si>
     <t>${limit}</t>
   </si>
   <si>
@@ -234,9 +228,6 @@
   </si>
   <si>
     <t>bDENtRlm1UchRTFGA3SP9MltOvCXnPff</t>
-  </si>
-  <si>
-    <t>${responseCode}</t>
   </si>
   <si>
     <t>SAMUNG123</t>
@@ -364,6 +355,9 @@
   </si>
   <si>
     <t>error message</t>
+  </si>
+  <si>
+    <t>LG</t>
   </si>
 </sst>
 </file>
@@ -534,58 +528,58 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -875,37 +869,37 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="28" t="s">
-        <v>80</v>
+      <c r="A7" s="27" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -935,7 +929,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
@@ -949,55 +943,55 @@
         <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="D3" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="D4" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="D5" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="D6" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="D7" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="D8" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="D9" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="D10" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="D11" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1005,15 +999,15 @@
     </row>
     <row r="13" spans="1:4">
       <c r="C13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="D14" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1048,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
@@ -1074,153 +1068,153 @@
         <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>24</v>
-      </c>
       <c r="E2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="43.5">
       <c r="D3" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="43.5">
       <c r="D4" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="43.5">
       <c r="D5" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="43.5">
       <c r="D6" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="43.5">
       <c r="D7" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.5">
       <c r="D8" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="29">
       <c r="D9" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>46</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="29">
       <c r="D10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="F10" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="58">
       <c r="D11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="11" t="s">
+      <c r="G11" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="43.5">
       <c r="F12" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>56</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1233,172 +1227,172 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{018945DD-5A3B-4201-AE04-C992905FCCE5}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="21.08984375" customWidth="1"/>
-    <col min="2" max="2" width="38.81640625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="38.81640625" style="16" customWidth="1"/>
     <col min="3" max="3" width="21.6328125" customWidth="1"/>
-    <col min="4" max="4" width="38.36328125" style="29" customWidth="1"/>
+    <col min="4" max="4" width="38.36328125" style="28" customWidth="1"/>
     <col min="5" max="5" width="36.6328125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="16.90625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="16.90625" style="32" customWidth="1"/>
     <col min="7" max="7" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="58">
       <c r="A2" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="32">
+        <v>200</v>
+      </c>
+      <c r="G2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="72.5">
+      <c r="B3" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="32">
+        <v>404</v>
+      </c>
+      <c r="G3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="43.5">
+      <c r="B4" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="F4" s="32">
+        <v>200</v>
+      </c>
+      <c r="G4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="58">
+      <c r="B5" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="D5" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F5" s="32">
+        <v>404</v>
+      </c>
+      <c r="G5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="43.5">
+      <c r="B6" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="32">
+        <v>404</v>
+      </c>
+      <c r="G6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="58">
+      <c r="B7" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="32">
         <v>200</v>
       </c>
-      <c r="G2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="72.5">
-      <c r="B3" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="33">
+      <c r="G7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="58">
+      <c r="B8" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="32">
+        <v>200</v>
+      </c>
+      <c r="G8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="58">
+      <c r="B9" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="32">
         <v>404</v>
       </c>
-      <c r="G3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="43.5">
-      <c r="B4" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" s="33">
-        <v>200</v>
-      </c>
-      <c r="G4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="58">
-      <c r="B5" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="33">
-        <v>404</v>
-      </c>
-      <c r="G5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="43.5">
-      <c r="B6" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" s="33">
-        <v>404</v>
-      </c>
-      <c r="G6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="58">
-      <c r="B7" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="33">
-        <v>200</v>
-      </c>
-      <c r="G7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="58">
-      <c r="B8" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F8" s="33">
-        <v>200</v>
-      </c>
-      <c r="G8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="58">
-      <c r="B9" s="29" t="s">
+      <c r="G9" t="s">
         <v>100</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F9" s="33">
-        <v>404</v>
-      </c>
-      <c r="G9" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1410,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7CF399-1BC0-4E90-AC7A-D91DF9E6B4DE}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1437,24 +1431,22 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>15</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B4" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{9D2BAD1F-EF5F-4572-BD7A-CC6B408C3168}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{934F7855-B6DA-41C9-88BC-EDE2383DA3A8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1471,11 +1463,11 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="28.81640625" customWidth="1"/>
-    <col min="2" max="3" width="6.7265625" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.90625" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.7265625" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.90625" style="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.08984375" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.08984375" style="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="58" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.7265625" customWidth="1"/>
@@ -1483,195 +1475,195 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33" customHeight="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="406">
+      <c r="A2" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="20">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20">
+        <v>1</v>
+      </c>
+      <c r="D2" s="20">
+        <v>3</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="20">
+        <v>1</v>
+      </c>
+      <c r="G2" s="20">
+        <v>200</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="406">
+      <c r="A3" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="18" t="s">
+      <c r="B3" s="19">
+        <v>1</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20">
+        <v>200</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="406">
+      <c r="A4" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="22">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20">
+        <v>2</v>
+      </c>
+      <c r="D4" s="20">
+        <v>3</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" s="30" t="s">
+      <c r="F4" s="20">
+        <v>1</v>
+      </c>
+      <c r="G4" s="20">
+        <v>200</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="406">
-      <c r="A2" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="21">
+    </row>
+    <row r="5" spans="1:11" ht="406">
+      <c r="A5" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="20">
+        <v>40</v>
+      </c>
+      <c r="G5" s="20">
+        <v>404</v>
+      </c>
+      <c r="H5" s="18"/>
+      <c r="I5" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="406">
+      <c r="A6" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="20">
+        <v>8</v>
+      </c>
+      <c r="C6" s="20">
+        <v>0</v>
+      </c>
+      <c r="D6" s="20">
+        <v>7</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="20">
         <v>1</v>
       </c>
-      <c r="C2" s="21">
-        <v>1</v>
-      </c>
-      <c r="D2" s="21">
-        <v>3</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="21">
-        <v>1</v>
-      </c>
-      <c r="G2" s="21">
-        <v>200</v>
-      </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="24" t="s">
+      <c r="G6" s="20">
+        <v>404</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="406">
-      <c r="A3" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="20">
-        <v>1</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21">
-        <v>200</v>
-      </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="J3" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="406">
-      <c r="A4" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="23">
-        <v>1</v>
-      </c>
-      <c r="C4" s="21">
-        <v>2</v>
-      </c>
-      <c r="D4" s="21">
-        <v>3</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="21">
-        <v>1</v>
-      </c>
-      <c r="G4" s="21">
-        <v>200</v>
-      </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="J4" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="406">
-      <c r="A5" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" s="21">
-        <v>40</v>
-      </c>
-      <c r="G5" s="21">
-        <v>404</v>
-      </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="J5" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="406">
-      <c r="A6" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="21">
-        <v>8</v>
-      </c>
-      <c r="C6" s="21">
-        <v>0</v>
-      </c>
-      <c r="D6" s="21">
-        <v>7</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="21">
-        <v>1</v>
-      </c>
-      <c r="G6" s="21">
-        <v>404</v>
-      </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="J6" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>76</v>
+      <c r="K6" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1683,8 +1675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62080006-4488-4B4E-9942-B6A50F18C1B5}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1701,42 +1693,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="14" t="s">
-        <v>64</v>
+      <c r="A1" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>60</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="F1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B2">
@@ -1748,8 +1740,8 @@
       <c r="D2">
         <v>3</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>65</v>
+      <c r="E2" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1757,36 +1749,36 @@
       <c r="G2">
         <v>404</v>
       </c>
-      <c r="J2" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>76</v>
+      <c r="J2" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>68</v>
+      <c r="A3" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" s="14"/>
+      <c r="E3" s="13"/>
       <c r="G3">
         <v>404</v>
       </c>
-      <c r="J3" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>76</v>
+      <c r="J3" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B4">
@@ -1798,8 +1790,8 @@
       <c r="D4">
         <v>20</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>69</v>
+      <c r="E4" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="F4">
         <v>40</v>
@@ -1808,36 +1800,36 @@
         <v>404</v>
       </c>
       <c r="J4" t="s">
-        <v>75</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="101.5">
-      <c r="A5" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" s="17">
+      <c r="A5" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="16">
         <v>8</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="16">
         <v>0</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="16">
         <v>7</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="17">
+      <c r="E5" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="16">
         <v>1</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="16">
         <v>404</v>
       </c>
-      <c r="K5" s="14" t="s">
-        <v>76</v>
+      <c r="K5" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>